<commit_message>
update batch upload of inbound & outbound
</commit_message>
<xml_diff>
--- a/aims_api.API/Template/Inbound/WhTransfer_Template.xlsx
+++ b/aims_api.API/Template/Inbound/WhTransfer_Template.xlsx
@@ -1,59 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mark\AIMS\aims_ui 05232023\src\assets\template\Inbound\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mark\AIMS\aims_api-main\aims_api-main\aims_api.API\Template\Inbound\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40E0D69-BF5F-48ED-8AB1-F74361264EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C185B10A-19F3-488C-9861-342B7D671934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1DD4515D-FDA9-4FFF-8A02-1003799E7F33}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PO_Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="30" uniqueCount="25">
   <si>
     <t>Reference Number</t>
   </si>
   <si>
+    <t>2nd Reference Number</t>
+  </si>
+  <si>
+    <t>Arrival Date</t>
+  </si>
+  <si>
+    <t>Arrival Date 2</t>
+  </si>
+  <si>
     <t>SKU</t>
   </si>
   <si>
-    <t>Order Qty.</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
-    <t>2nd Reference Number</t>
-  </si>
-  <si>
-    <t>Arrival Date</t>
+    <t>Carrier Id</t>
   </si>
   <si>
     <t>Carrier Name</t>
@@ -62,35 +54,59 @@
     <t>Carrier Address</t>
   </si>
   <si>
+    <t>Carrier Contact</t>
+  </si>
+  <si>
     <t>Carrier Email</t>
   </si>
   <si>
-    <t>Arrival Date 2</t>
-  </si>
-  <si>
-    <t>Warehouse Name</t>
-  </si>
-  <si>
-    <t>Warehouse Address</t>
-  </si>
-  <si>
-    <t>Warehouse Contact No</t>
-  </si>
-  <si>
-    <t>Warehouse Email</t>
-  </si>
-  <si>
-    <t>Carrier Contact No</t>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Modified By</t>
+  </si>
+  <si>
+    <t>2023-06-15T15:30:00Z</t>
+  </si>
+  <si>
+    <t>2023-06-29T15:30:00Z</t>
+  </si>
+  <si>
+    <t>SKU-00003</t>
+  </si>
+  <si>
+    <t>DEV-Mark</t>
+  </si>
+  <si>
+    <t>SKU-00001</t>
+  </si>
+  <si>
+    <t>Warehouse Contact</t>
   </si>
   <si>
     <t>Transfer Date</t>
+  </si>
+  <si>
+    <t>Warehouse From</t>
+  </si>
+  <si>
+    <t>Expected Qty.</t>
+  </si>
+  <si>
+    <t>Warehouse From Id</t>
+  </si>
+  <si>
+    <t>Warehouse From Address</t>
+  </si>
+  <si>
+    <t>Warehouse From Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,32 +114,521 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color rgb="FF7F7F7F"/>
+      </start>
+      <end style="thin">
+        <color rgb="FF7F7F7F"/>
+      </end>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color rgb="FF3F3F3F"/>
+      </start>
+      <end style="thin">
+        <color rgb="FF3F3F3F"/>
+      </end>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="double">
+        <color rgb="FF3F3F3F"/>
+      </start>
+      <end style="double">
+        <color rgb="FF3F3F3F"/>
+      </end>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color rgb="FFB2B2B2"/>
+      </start>
+      <end style="thin">
+        <color rgb="FFB2B2B2"/>
+      </end>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +644,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -292,25 +797,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -318,25 +823,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -349,21 +854,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -377,7 +882,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -389,32 +894,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -434,78 +939,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3842DF-7784-4D0D-BA02-33F3841C67AC}">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" customWidth="1"/>
-    <col min="14" max="14" width="10.7265625" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>5223443</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="G2">
+        <v>500</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5223444</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" t="s">
-        <v>3</v>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>